<commit_message>
implement programming language syntax highlighting
</commit_message>
<xml_diff>
--- a/scraping/declarations.xlsx
+++ b/scraping/declarations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Year4\From Idea to App\Final Project\DeveloCoop\scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6D7F64-DFD4-47A5-BF03-7D8824DF4813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7517CA7-AE2B-48AD-B464-4FF3EECCFEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -913,16 +913,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">def stockBuySell(A, N ):
-	"""
-	type N: int
-	type A: List[int]
-	type return: List[int]
-	"""
-	pass
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">def trappingWater(arr, N):
 	"""
 	type N: int
@@ -1321,6 +1311,16 @@
 	type return: List[int]
 	"""
 	pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def stockBuySell(A, N):
+	"""
+	type N: int
+	type A: List[int]
+	type return: List[int]
+	"""
+	pass
+</t>
   </si>
 </sst>
 </file>
@@ -1702,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,7 +2252,7 @@
         <v>61</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>162</v>
+        <v>203</v>
       </c>
       <c r="C60" s="1"/>
     </row>
@@ -2261,7 +2261,7 @@
         <v>62</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C61" s="1"/>
     </row>
@@ -2270,7 +2270,7 @@
         <v>63</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C62" s="1"/>
     </row>
@@ -2279,7 +2279,7 @@
         <v>64</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C63" s="1"/>
     </row>
@@ -2288,7 +2288,7 @@
         <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C64" s="1"/>
     </row>
@@ -2297,7 +2297,7 @@
         <v>66</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C65" s="1"/>
     </row>
@@ -2306,7 +2306,7 @@
         <v>67</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C66" s="1"/>
     </row>
@@ -2315,7 +2315,7 @@
         <v>68</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C67" s="1"/>
     </row>
@@ -2324,7 +2324,7 @@
         <v>69</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C68" s="1"/>
     </row>
@@ -2333,7 +2333,7 @@
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C69" s="1"/>
     </row>
@@ -2342,7 +2342,7 @@
         <v>71</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C70" s="1"/>
     </row>
@@ -2351,7 +2351,7 @@
         <v>72</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C71" s="1"/>
     </row>
@@ -2360,7 +2360,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C72" s="1"/>
     </row>
@@ -2369,7 +2369,7 @@
         <v>74</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C73" s="1"/>
     </row>
@@ -2378,7 +2378,7 @@
         <v>75</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C74" s="1"/>
     </row>
@@ -2387,7 +2387,7 @@
         <v>76</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C75" s="1"/>
     </row>
@@ -2396,7 +2396,7 @@
         <v>77</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C76" s="1"/>
     </row>
@@ -2405,7 +2405,7 @@
         <v>78</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C77" s="1"/>
     </row>
@@ -2414,7 +2414,7 @@
         <v>79</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C78" s="1"/>
     </row>
@@ -2423,7 +2423,7 @@
         <v>80</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C79" s="1"/>
     </row>
@@ -2432,7 +2432,7 @@
         <v>81</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C80" s="1"/>
     </row>
@@ -2441,7 +2441,7 @@
         <v>82</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C81" s="1"/>
     </row>
@@ -2450,7 +2450,7 @@
         <v>83</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C82" s="1"/>
     </row>
@@ -2459,7 +2459,7 @@
         <v>84</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C83" s="1"/>
     </row>
@@ -2468,7 +2468,7 @@
         <v>85</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C84" s="1"/>
     </row>
@@ -2477,7 +2477,7 @@
         <v>86</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C85" s="1"/>
     </row>
@@ -2486,7 +2486,7 @@
         <v>87</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C86" s="1"/>
     </row>
@@ -2495,7 +2495,7 @@
         <v>88</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C87" s="1"/>
     </row>
@@ -2504,7 +2504,7 @@
         <v>89</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C88" s="1"/>
     </row>
@@ -2513,7 +2513,7 @@
         <v>90</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C89" s="1"/>
     </row>
@@ -2522,7 +2522,7 @@
         <v>91</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C90" s="1"/>
     </row>
@@ -2531,7 +2531,7 @@
         <v>92</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C91" s="1"/>
     </row>
@@ -2540,7 +2540,7 @@
         <v>93</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C92" s="1"/>
     </row>
@@ -2549,7 +2549,7 @@
         <v>94</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C93" s="1"/>
     </row>
@@ -2558,7 +2558,7 @@
         <v>95</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C94" s="1"/>
     </row>
@@ -2567,7 +2567,7 @@
         <v>96</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C95" s="1"/>
     </row>
@@ -2576,7 +2576,7 @@
         <v>97</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C96" s="1"/>
     </row>
@@ -2585,7 +2585,7 @@
         <v>98</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C97" s="1"/>
     </row>
@@ -2594,7 +2594,7 @@
         <v>99</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C98" s="1"/>
     </row>
@@ -2603,7 +2603,7 @@
         <v>100</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C99" s="1"/>
     </row>
@@ -2612,7 +2612,7 @@
         <v>101</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C100" s="1"/>
     </row>
@@ -2621,7 +2621,7 @@
         <v>102</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C101" s="1"/>
     </row>

</xml_diff>

<commit_message>
replace TABS with SPACES in DB declarations
</commit_message>
<xml_diff>
--- a/scraping/declarations.xlsx
+++ b/scraping/declarations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Year4\From Idea to App\Final Project\DeveloCoop\scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7517CA7-AE2B-48AD-B464-4FF3EECCFEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BE2972-03C5-465E-8D4F-4A5A1330EAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,14 +331,11 @@
     <t>Common Elements</t>
   </si>
   <si>
-    <t>3 functions</t>
-  </si>
-  <si>
     <t>def printPat(n):
-	"""
-	type n: int
-	"""
-	pass</t>
+    """
+    type n: int
+    """
+    pass</t>
   </si>
   <si>
     <t xml:space="preserve">def getTable(N):
@@ -639,688 +636,691 @@
   </si>
   <si>
     <t xml:space="preserve">def trailingZeroes(N):
-	"""
-	type N: int
-	type return: int
-	"""
-	pass
+    """
+    type N: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def getAngle(H, M):
-	"""
-	type H: int
-	type M: int
-	type return: int
-	"""
-	pass
+    """
+    type H: int
+    type M: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def noOfOpenDoors(N):
-	"""
-	type N: int
-	type return: int
-	"""
-	pass
+    """
+    type N: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def isTriangular(N):
-	"""
-	type N: int
-	type return: int
-	"""
-	pass
+    """
+    type N: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def nthEvenFibonacci(n):
-	"""
-	type n: int
-	type return: int
-	"""
-	pass
+    """
+    type n: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def fibonacciDigits(N):
-	"""
-	type N: int
-	type return: int
-	"""
-	pass
+    """
+    type N: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def squaresInMatrix(m, n):
-	"""
-	type m: int
-	type n: int
-	type return: int
-	"""
-	pass
+    """
+    type m: int
+    type n: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def getDayOfWeek(d, m, y):
-	"""
-	type d: int
-	type m: int
-	type y: int
-	type return: str
-	"""
-	pass
+    """
+    type d: int
+    type m: int
+    type y: int
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def searchEle(arr, x):
-	"""
-	type arr: List[int]
-	type x: int
-	type return: bool
-	"""
-	pass
+    """
+    type arr: List[int]
+    type x: int
+    type return: bool
+    """
+    pass
 def insertEle(arr, y, yi):
-	"""
-	type arr: List[int]
-	type y: int
-	type yi: int
-	type return: int
-	"""
-	pass
+    """
+    type arr: List[int]
+    type y: int
+    type yi: int
+    type return: int
+    """
+    pass
 def deleteEle(arr, z):
-	"""
-	type arr: List[int]
-	type z: int
-	type return: int
-	"""
-	pass
+    """
+    type arr: List[int]
+    type z: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def printAl(arr):
-	"""
-	type arr: List[int]
-	"""
-	pass
+    """
+    type arr: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def get_min_and_max(arr):
-	"""
-	type arr: List[int]
-	type return: tuple[int]
-	"""
-	pass
+    """
+    type arr: List[int]
+    type return: tuple[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def print2largest(arr):
-	"""
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def rotateArr( arr, d, n):
-	"""
-	type n: int
-	type d: int
-	type arr: List[int]
-	type return: List[int]
-	"""
-	pass
+    """
+    type n: int
+    type d: int
+    type arr: List[int]
+    type return: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def countOfElements(x, arr):
-	"""
-	type n: int
-	type d: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type n: int
+    type d: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def remove_duplicate(arr):
-	"""
-	type arr: List[int]
-	type return: List[int]
-	"""
-	pass
+    """
+    type arr: List[int]
+    type return: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def findNumberOfTriangles(arr, n):
-	"""
-	type n: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type n: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def leaders(n, arr):
-	"""
-	type n: int
-	type arr: List[int]
-	type return: List[int]
-	"""
-	pass
+    """
+    type n: int
+    type arr: List[int]
+    type return: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def minDist( a, n, x, y):
-	"""
-	type n: int
-	type a: List[int]
-	type x: int
-	type y: int
-	type return: int
-	"""
-	pass
+    """
+    type n: int
+    type a: List[int]
+    type x: int
+    type y: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def find3Numbers(arr):
-	"""
-	type arr: List[int]
-	type return: List[int]
-	"""
-	pass
+    """
+    type arr: List[int]
+    type return: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def findSubarray(n, a):
-	"""
-	type n: int
-	type a: List[int]
-	type return: List[int]
-	"""
-	pass
+    """
+    type n: int
+    type a: List[int]
+    type return: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def majorityElement(A, N):
-	"""
-	type N: int
-	type A: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type N: int
+    type A: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def convertToWave(n, arr):
-	"""
-	type n: int
-	type arr: List[int]
-	"""
-	pass
+    """
+    type n: int
+    type arr: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def maxIndexDiff(arr):
-	"""
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def max_sum_path(arr1, arr2):
-	"""
-	type arr1: List[int]
-	type arr2: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type arr1: List[int]
+    type arr2: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def productExceptSelf(nums):
-	"""
-	type nums: List[int]
-	type return: List[int]
-	"""
-	pass
+    """
+    type nums: List[int]
+    type return: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def duplicates(arr):
-	"""
-	type arr: List[int]
-	type return: List[int]
-	"""
-	pass
+    """
+    type arr: List[int]
+    type return: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def findTwoElements(arr, n):
-	"""
-	type n: int
-	type arr: List[int]
-	type return: List[int]
-	"""
-	pass
+    """
+    type n: int
+    type arr: List[int]
+    type return: List[int]
+    """
+    pass
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def stockBuySell(A, N):
+    """
+    type N: int
+    type A: List[int]
+    type return: List[int]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def trappingWater(arr, N):
-	"""
-	type N: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type N: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def countPair(k, arr):
-	"""
-	type k: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type k: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def findMinDiff(A, N, M):
-	"""
-	type N: int
-	type M: int
-	type A: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type N: int
+    type M: int
+    type A: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def findLongestConseqSubseq(arr, N):
-	"""
-	type N: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type N: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def threeWayPartition(array, a, b):
-	"""
-	type array: List[int]
-	type a: int
-	type b: int
-	"""
-	pass
+    """
+    type array: List[int]
+    type a: int
+    type b: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def isPalindrome(S):
-	"""
-	type S: str
-	type return: int
-	"""
-	pass
+    """
+    type S: str
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def isAnagram(a, b):
-	"""
-	type a: str
-	type b: str
-	type return: bool
-	"""
-	pass
+    """
+    type a: str
+    type b: str
+    type return: bool
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def isPossible(S):
-	"""
-	type S: str
-	type return: int
-	"""
-	pass
+    """
+    type S: str
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def transform(str):
-	"""
-	type str: str
-	type return: str
-	"""
-	pass
+    """
+    type str: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def reverseSort(str):
-	"""
-	type str: str
-	type return: str
-	"""
-	pass
+    """
+    type str: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def merge(S1, S2):
-	"""
-	type S1: str
-	type S2: str
-	type return: str
-	"""
-	pass
+    """
+    type S1: str
+    type S2: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def isGoodOrBad(S):
-	"""
-	type S: str
-	type return: int
-	"""
-	pass
+    """
+    type S: str
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def extractMaximum(S):
-	"""
-	type S: str
-	type return: int
-	"""
-	pass
+    """
+    type S: str
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def reverseWords(S):
-	"""
-	type S: str
-	type return: str
-	"""
-	pass
+    """
+    type S: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def strstr(s, x):
-	"""
-	type s: str
-	type x: str
-	type return: int
-	"""
-	pass
+    """
+    type s: str
+    type x: str
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def isSubSequence(A, B):
-	"""
-	type A: str
-	type B: str
-	type return: bool
-	"""
-	pass
+    """
+    type A: str
+    type B: str
+    type return: bool
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def areRotations(s1, s2):
-	"""
-	type s1: str
-	type s2: str
-	type return: bool
-	"""
-	pass
+    """
+    type s1: str
+    type s2: str
+    type return: bool
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def areKAnagrams(str1, str2, k):
-	"""
-	type s1: str
-	type s2: str
-	type k: int
-	type return: int
-	"""
-	pass
+    """
+    type s1: str
+    type s2: str
+    type k: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def uncommonChars(A, B):
-	"""
-	type A: str
-	type B: str
-	type return: str
-	"""
-	pass
+    """
+    type A: str
+    type B: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def remAnagram(S1, S2):
-	"""
-	type S1: str
-	type S2: str
-	type return: int
-	"""
-	pass
+    """
+    type S1: str
+    type S2: str
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def nonRepeatingCharacter(s):
-	"""
-	type s: str
-	type return: str
-	"""
-	pass
+    """
+    type s: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def longestSubstrDistinctChars(S):
-	"""
-	type S: str
-	type return: int
-	"""
-	pass
+    """
+    type S: str
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def LongestPalindromeSubString(text):
-	"""
-	type text: List[str]
-	type return: List[str]
-	"""
-	pass
+    """
+    type text: List[str]
+    type return: List[str]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def kthCharacter(m, n, k):
-	"""
-	type m: int
-	type n: int
-	type k: int
-	type return: str
-	"""
-	pass
+    """
+    type m: int
+    type n: int
+    type k: int
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def smallestWindow(S, P):
-	"""
-	type S: str
-	type P: str
-	type return: str
-	"""
-	pass
+    """
+    type S: str
+    type P: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def addBinary(A, B):
-	"""
-	type A: str
-	type B: str
-	type return: str
-	"""
-	pass
+    """
+    type A: str
+    type B: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def multiplyStrings(s1, s2):
-	"""
-	type s1: str
-	type s2: str
-	type return: str
-	"""
-	pass
+    """
+    type s1: str
+    type s2: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def roundToNearest(str):
-	"""
-	type str: str
-	type return: str
-	"""
-	pass
+    """
+    type str: str
+    type return: str
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def search(k, arr):
-	"""
-	type k: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type k: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def nullPoints(N, M, getAnswer):
-	"""
-	type N: int
-	type M: List[float]
-	type getAnswer: List[float]
-	"""
-	pass
+    """
+    type N: int
+    type M: List[float]
+    type getAnswer: List[float]
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def binarysearch(arr, k):
-	"""
-	type k: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type k: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def findFloor( arr, n, x):
-	"""
-	type n: int
-	type x: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type n: int
+    type x: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def count(Arr, N, X):
-	"""
-	type N: int
-	type X: int
-	type Arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type N: int
+    type X: int
+    type Arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def search(arr, key):
-	"""
-	type arr: List[int]
-	type key: int
-	type return: int
-	"""
-	pass
+    """
+    type arr: List[int]
+    type key: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def missingNumber(n, arr):
-	"""
-	type n: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type n: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def findMissing(arr):
-	"""
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def floorSqrt(n):
-	"""
-	type n: int
-	type return: int
-	"""
-	pass
+    """
+    type n: int
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def lastIndex(s):
-	"""
-	type s: str
-	type return: int
-	"""
-	pass
+    """
+    type s: str
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t xml:space="preserve">def peakElement( arr, n):
-	"""
-	type n: int
-	type arr: List[int]
-	type return: int
-	"""
-	pass
+    """
+    type n: int
+    type arr: List[int]
+    type return: int
+    """
+    pass
 </t>
   </si>
   <si>
     <t>def findPages(n, arr, m):
-	"""
-	type n: int
-	type arr: List[int]
-	type m: int
-	type return: int
-	"""
-	pass</t>
+    """
+    type n: int
+    type arr: List[int]
+    type m: int
+    type return: int
+    """
+    pass</t>
   </si>
   <si>
     <t>def common_element(V1, V2):
-	"""
-	type V1: List[int]
-	type V2: List[int]
-	type return: List[int]
-	"""
-	pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def stockBuySell(A, N):
-	"""
-	type N: int
-	type A: List[int]
-	type return: List[int]
-	"""
-	pass
-</t>
+    """
+    type V1: List[int]
+    type V2: List[int]
+    type return: List[int]
+    """
+    pass</t>
+  </si>
+  <si>
+    <t>3 functions</t>
   </si>
 </sst>
 </file>
@@ -1344,18 +1344,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1385,15 +1379,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1702,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,921 +1703,821 @@
     <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
         <v>116</v>
       </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
         <v>128</v>
       </c>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
         <v>129</v>
       </c>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
         <v>130</v>
       </c>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="1" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" ht="225" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
         <v>133</v>
       </c>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
         <v>134</v>
       </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="1" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="1" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="1" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
         <v>137</v>
       </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="1" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
         <v>138</v>
       </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="1" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
         <v>139</v>
       </c>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="1" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
         <v>140</v>
       </c>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="1" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
         <v>141</v>
       </c>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="1" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
         <v>142</v>
       </c>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" ht="375" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" t="s">
         <v>143</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="1" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" t="s">
         <v>144</v>
       </c>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="1" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
         <v>145</v>
       </c>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" s="1" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
         <v>146</v>
       </c>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="1" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
         <v>147</v>
       </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="1" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
         <v>148</v>
       </c>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="1" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
         <v>149</v>
       </c>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="1" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
         <v>150</v>
       </c>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="1" t="s">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
         <v>151</v>
       </c>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="1" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
         <v>152</v>
       </c>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="1" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" t="s">
         <v>153</v>
       </c>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="1" t="s">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
         <v>154</v>
       </c>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="1" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="s">
         <v>155</v>
       </c>
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="1" t="s">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" t="s">
         <v>156</v>
       </c>
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="1" t="s">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" t="s">
         <v>157</v>
       </c>
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" s="1" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
         <v>158</v>
       </c>
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="1" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
         <v>159</v>
       </c>
-      <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" s="1" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
         <v>160</v>
       </c>
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" s="1" t="s">
+    </row>
+    <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>162</v>
       </c>
-      <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>163</v>
       </c>
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>164</v>
       </c>
-      <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>165</v>
       </c>
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>166</v>
       </c>
-      <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    </row>
+    <row r="66" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>67</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>168</v>
       </c>
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>169</v>
       </c>
-      <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>170</v>
       </c>
-      <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>171</v>
       </c>
-      <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>172</v>
       </c>
-      <c r="C71" s="1"/>
-    </row>
-    <row r="72" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>173</v>
       </c>
-      <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>74</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>174</v>
       </c>
-      <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>175</v>
       </c>
-      <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>176</v>
       </c>
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>77</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>177</v>
       </c>
-      <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>78</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>178</v>
       </c>
-      <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>79</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>179</v>
       </c>
-      <c r="C78" s="1"/>
-    </row>
-    <row r="79" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>80</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>81</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>181</v>
       </c>
-      <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>82</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>182</v>
       </c>
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>183</v>
       </c>
-      <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>84</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" t="s">
         <v>184</v>
       </c>
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>85</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>185</v>
       </c>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>86</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" t="s">
         <v>186</v>
       </c>
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>87</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>187</v>
       </c>
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>88</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>188</v>
       </c>
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>89</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>189</v>
       </c>
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>90</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" t="s">
         <v>190</v>
       </c>
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>91</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>191</v>
       </c>
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    </row>
+    <row r="91" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>92</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>93</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>193</v>
       </c>
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>94</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>194</v>
       </c>
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>95</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>195</v>
       </c>
-      <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>96</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>196</v>
       </c>
-      <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>97</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>197</v>
       </c>
-      <c r="C96" s="1"/>
-    </row>
-    <row r="97" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>98</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" t="s">
         <v>198</v>
       </c>
-      <c r="C97" s="1"/>
-    </row>
-    <row r="98" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>99</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" t="s">
         <v>199</v>
       </c>
-      <c r="C98" s="1"/>
-    </row>
-    <row r="99" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" t="s">
         <v>200</v>
       </c>
-      <c r="C99" s="1"/>
-    </row>
-    <row r="100" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>101</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" t="s">
         <v>201</v>
       </c>
-      <c r="C100" s="1"/>
-    </row>
-    <row r="101" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>102</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" t="s">
         <v>202</v>
       </c>
-      <c r="C101" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>